<commit_message>
im going to bed now
</commit_message>
<xml_diff>
--- a/TEMP/table.xlsx
+++ b/TEMP/table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>Parts quote: 22135479</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Unnamed: 9</t>
   </si>
   <si>
-    <t>Parts</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>Buy</t>
-  </si>
-  <si>
     <t>$450.00</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
   </si>
   <si>
     <t>$1.80</t>
-  </si>
-  <si>
-    <t>Sell</t>
   </si>
   <si>
     <t>Price</t>
@@ -581,7 +572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,112 +611,139 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="H2" t="s">
-        <v>51</v>
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>10</v>
+      <c r="B3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>11</v>
       </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
       <c r="F4" t="s">
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" t="s">
-        <v>26</v>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -733,79 +751,70 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -819,29 +828,32 @@
         <v>39</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>427</v>
       </c>
       <c r="E14">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
@@ -850,32 +862,29 @@
         <v>40</v>
       </c>
       <c r="D16">
-        <v>427</v>
+        <v>62</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="G16" t="s">
         <v>49</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17">
-        <v>84</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
@@ -884,24 +893,24 @@
         <v>41</v>
       </c>
       <c r="D18">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="E18">
-        <v>136</v>
+        <v>228</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -912,64 +921,33 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D20">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>228</v>
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>41</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" t="s">
-        <v>45</v>
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>